<commit_message>
SVN (res) commit #2589 by scriswellwsf       misc 2025 rule/UI updates
</commit_message>
<xml_diff>
--- a/RulesetSrc/T24SFam/To-Docu/T24RClimateZoneCodeBaselines.xlsx
+++ b/RulesetSrc/T24SFam/To-Docu/T24RClimateZoneCodeBaselines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN-CBECC-Res-20250331\RulesetDev\Rulesets\CA Res\Rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBECC-Res\SVNv2\trunk\RulesetSrc\T24SFam\To-Docu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE57DF4D-2F22-45B5-9055-1DB2B74B51D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B73019-1424-4DF5-9F8D-869E81E5A3CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1005" yWindow="2085" windowWidth="24570" windowHeight="14865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="T24RClimateZoneCodeBaselines" sheetId="1" r:id="rId1"/>
@@ -2052,7 +2052,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>based on table &amp; formula 7/19/23</t>
         </r>
@@ -2066,7 +2066,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>SAC 07/21/23:</t>
         </r>
@@ -2075,7 +2075,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 updated for 2025 prescrip PV </t>
@@ -2102,7 +2102,18 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-updated for 2025 code vintage</t>
+updated for 2025 code vintage
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>NOT USED as of 6/2025</t>
         </r>
       </text>
     </comment>
@@ -3632,7 +3643,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="37" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3886,19 +3897,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="39">
@@ -4948,8 +4946,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FF412"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="C144" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="F347" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="C144" sqref="C144"/>
+      <selection pane="topRight" activeCell="F144" sqref="F144"/>
+      <selection pane="bottomLeft" activeCell="C149" sqref="C149"/>
+      <selection pane="bottomRight" activeCell="U382" sqref="U382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -61239,7 +61241,7 @@
       <c r="CK362" s="13"/>
       <c r="CM362" s="13"/>
     </row>
-    <row r="363" spans="3:91" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="3:91" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="C363" s="3">
         <v>1</v>
       </c>
@@ -61480,7 +61482,7 @@
       <c r="CK363" s="13"/>
       <c r="CM363" s="13"/>
     </row>
-    <row r="364" spans="3:91" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="3:91" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="C364" s="3">
         <v>2</v>
       </c>
@@ -61733,7 +61735,7 @@
       <c r="CK364" s="13"/>
       <c r="CM364" s="13"/>
     </row>
-    <row r="365" spans="3:91" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="3:91" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="C365" s="3">
         <v>3</v>
       </c>
@@ -61986,7 +61988,7 @@
       <c r="CK365" s="13"/>
       <c r="CM365" s="13"/>
     </row>
-    <row r="366" spans="3:91" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="3:91" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="C366" s="3">
         <v>4</v>
       </c>
@@ -62239,7 +62241,7 @@
       <c r="CK366" s="13"/>
       <c r="CM366" s="13"/>
     </row>
-    <row r="367" spans="3:91" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="3:91" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="C367" s="3">
         <v>5</v>
       </c>
@@ -62492,7 +62494,7 @@
       <c r="CK367" s="13"/>
       <c r="CM367" s="13"/>
     </row>
-    <row r="368" spans="3:91" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="3:91" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="C368" s="3">
         <v>6</v>
       </c>
@@ -62744,7 +62746,7 @@
       <c r="CK368" s="13"/>
       <c r="CM368" s="13"/>
     </row>
-    <row r="369" spans="1:162" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:162" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="C369" s="3">
         <v>7</v>
       </c>
@@ -62995,7 +62997,7 @@
       <c r="CK369" s="13"/>
       <c r="CM369" s="13"/>
     </row>
-    <row r="370" spans="1:162" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:162" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="C370" s="3">
         <v>8</v>
       </c>
@@ -63246,7 +63248,7 @@
       <c r="CK370" s="13"/>
       <c r="CM370" s="13"/>
     </row>
-    <row r="371" spans="1:162" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:162" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="C371" s="3">
         <v>9</v>
       </c>
@@ -63499,7 +63501,7 @@
       <c r="CK371" s="13"/>
       <c r="CM371" s="13"/>
     </row>
-    <row r="372" spans="1:162" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:162" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="C372" s="3">
         <v>10</v>
       </c>
@@ -63752,7 +63754,7 @@
       <c r="CK372" s="13"/>
       <c r="CM372" s="13"/>
     </row>
-    <row r="373" spans="1:162" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:162" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="C373" s="3">
         <v>11</v>
       </c>
@@ -64005,7 +64007,7 @@
       <c r="CK373" s="13"/>
       <c r="CM373" s="13"/>
     </row>
-    <row r="374" spans="1:162" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:162" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="C374" s="3">
         <v>12</v>
       </c>
@@ -64258,7 +64260,7 @@
       <c r="CK374" s="13"/>
       <c r="CM374" s="13"/>
     </row>
-    <row r="375" spans="1:162" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:162" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="C375" s="3">
         <v>13</v>
       </c>
@@ -64511,7 +64513,7 @@
       <c r="CK375" s="13"/>
       <c r="CM375" s="13"/>
     </row>
-    <row r="376" spans="1:162" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:162" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="C376" s="3">
         <v>14</v>
       </c>
@@ -64764,7 +64766,7 @@
       <c r="CK376" s="13"/>
       <c r="CM376" s="13"/>
     </row>
-    <row r="377" spans="1:162" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:162" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="C377" s="3">
         <v>15</v>
       </c>
@@ -65017,7 +65019,7 @@
       <c r="CK377" s="13"/>
       <c r="CM377" s="13"/>
     </row>
-    <row r="378" spans="1:162" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:162" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="C378" s="3">
         <v>16</v>
       </c>
@@ -65651,7 +65653,7 @@
       <c r="R380" s="3">
         <v>0.1</v>
       </c>
-      <c r="S380" s="3">
+      <c r="S380" s="30">
         <v>21</v>
       </c>
       <c r="T380" s="3">
@@ -65897,7 +65899,7 @@
       <c r="R381" s="3">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="S381" s="3">
+      <c r="S381" s="30">
         <v>21</v>
       </c>
       <c r="T381" s="3">
@@ -66152,7 +66154,7 @@
       <c r="R382" s="3">
         <v>0.1</v>
       </c>
-      <c r="S382" s="3">
+      <c r="S382" s="30">
         <v>21</v>
       </c>
       <c r="T382" s="3">
@@ -66407,7 +66409,7 @@
       <c r="R383" s="3">
         <v>0.09</v>
       </c>
-      <c r="S383" s="3">
+      <c r="S383" s="30">
         <v>21</v>
       </c>
       <c r="T383" s="3">
@@ -66662,7 +66664,7 @@
       <c r="R384" s="3">
         <v>0.11</v>
       </c>
-      <c r="S384" s="3">
+      <c r="S384" s="30">
         <v>21</v>
       </c>
       <c r="T384" s="3">
@@ -66917,7 +66919,7 @@
       <c r="R385" s="3">
         <v>0.04</v>
       </c>
-      <c r="S385" s="3">
+      <c r="S385" s="30">
         <v>20</v>
       </c>
       <c r="T385" s="3">
@@ -67171,7 +67173,7 @@
       <c r="R386" s="3">
         <v>0.04</v>
       </c>
-      <c r="S386" s="3">
+      <c r="S386" s="30">
         <v>18</v>
       </c>
       <c r="T386" s="3">
@@ -67425,7 +67427,7 @@
       <c r="R387" s="3">
         <v>0.1</v>
       </c>
-      <c r="S387" s="3">
+      <c r="S387" s="30">
         <v>21</v>
       </c>
       <c r="T387" s="3">
@@ -67679,7 +67681,7 @@
       <c r="R388" s="3">
         <v>0.1</v>
       </c>
-      <c r="S388" s="3">
+      <c r="S388" s="30">
         <v>21</v>
       </c>
       <c r="T388" s="3">
@@ -67934,7 +67936,7 @@
       <c r="R389" s="3">
         <v>0.1</v>
       </c>
-      <c r="S389" s="3">
+      <c r="S389" s="30">
         <v>21</v>
       </c>
       <c r="T389" s="3">
@@ -68189,7 +68191,7 @@
       <c r="R390" s="3">
         <v>0.1</v>
       </c>
-      <c r="S390" s="3">
+      <c r="S390" s="30">
         <v>21</v>
       </c>
       <c r="T390" s="3">
@@ -68444,7 +68446,7 @@
       <c r="R391" s="3">
         <v>0.1</v>
       </c>
-      <c r="S391" s="3">
+      <c r="S391" s="30">
         <v>21</v>
       </c>
       <c r="T391" s="3">
@@ -68699,7 +68701,7 @@
       <c r="R392" s="3">
         <v>0.1</v>
       </c>
-      <c r="S392" s="3">
+      <c r="S392" s="30">
         <v>21</v>
       </c>
       <c r="T392" s="3">
@@ -68954,7 +68956,7 @@
       <c r="R393" s="3">
         <v>0.1</v>
       </c>
-      <c r="S393" s="3">
+      <c r="S393" s="30">
         <v>21</v>
       </c>
       <c r="T393" s="3">
@@ -69209,7 +69211,7 @@
       <c r="R394" s="3">
         <v>0.09</v>
       </c>
-      <c r="S394" s="3">
+      <c r="S394" s="30">
         <v>21</v>
       </c>
       <c r="T394" s="3">
@@ -69464,7 +69466,7 @@
       <c r="R395" s="83">
         <v>0.12</v>
       </c>
-      <c r="S395" s="83">
+      <c r="S395" s="84">
         <v>21</v>
       </c>
       <c r="T395" s="83">

</xml_diff>

<commit_message>
Issue #396 Additional table lookup updates
</commit_message>
<xml_diff>
--- a/RulesetSrc/T24SFam/To-Docu/T24RClimateZoneCodeBaselines.xlsx
+++ b/RulesetSrc/T24SFam/To-Docu/T24RClimateZoneCodeBaselines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\NOR-Codes-Stds\CBECC-Dev\RulesetSrc\T24SFam\To-Docu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACE0A84-C88F-4A3D-AE2C-944B98ACD077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF610FB-563D-4D5C-BFB8-0BB74E47B3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,6 +39,10 @@
     <author>tc={9B6BED9D-5D9F-45CA-BF02-2B591E00AB15}</author>
     <author>tc={8E6D4CA8-79C7-4082-B9FF-A694577BC82F}</author>
     <author>tc={B702ED2D-EA27-4105-9F3D-EEB895251933}</author>
+    <author>tc={5A2AFC92-DD15-4AE2-A916-B8A6D20139CD}</author>
+    <author>tc={EC86CE9C-E40B-4C6A-A9B2-7780F895100E}</author>
+    <author>tc={CFBF76F3-508B-478A-AA3B-D827B9843997}</author>
+    <author>tc={364B9DA7-9101-467F-9DFB-6A79815EFFAC}</author>
     <author>tc={FC2E1ABC-F00F-493D-803C-4517A7E565B1}</author>
     <author>tc={2E9A3BF3-11C4-488F-BCDE-80182BAD232A}</author>
     <author>tc={030E6257-8D2E-4479-8789-601A0BD01F26}</author>
@@ -2421,7 +2425,39 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH397" authorId="6" shapeId="0" xr:uid="{FC2E1ABC-F00F-493D-803C-4517A7E565B1}">
+    <comment ref="AW386" authorId="6" shapeId="0" xr:uid="{5A2AFC92-DD15-4AE2-A916-B8A6D20139CD}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    0.2 =&gt; 0.1 per Issue 396</t>
+      </text>
+    </comment>
+    <comment ref="AX386" authorId="7" shapeId="0" xr:uid="{EC86CE9C-E40B-4C6A-A9B2-7780F895100E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    0.63 =&gt; 0.1 per Issue 396 Table 150.1-A</t>
+      </text>
+    </comment>
+    <comment ref="AW390" authorId="8" shapeId="0" xr:uid="{CFBF76F3-508B-478A-AA3B-D827B9843997}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    0.2 =&gt; 0.1 per Issue 396</t>
+      </text>
+    </comment>
+    <comment ref="AW391" authorId="9" shapeId="0" xr:uid="{364B9DA7-9101-467F-9DFB-6A79815EFFAC}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    0.2 =&gt; 0.1 per Issue 396</t>
+      </text>
+    </comment>
+    <comment ref="AH397" authorId="10" shapeId="0" xr:uid="{FC2E1ABC-F00F-493D-803C-4517A7E565B1}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2429,7 +2465,7 @@
     Tic #1396</t>
       </text>
     </comment>
-    <comment ref="AS397" authorId="7" shapeId="0" xr:uid="{2E9A3BF3-11C4-488F-BCDE-80182BAD232A}">
+    <comment ref="AS397" authorId="11" shapeId="0" xr:uid="{2E9A3BF3-11C4-488F-BCDE-80182BAD232A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2753,7 +2789,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG416" authorId="8" shapeId="0" xr:uid="{030E6257-8D2E-4479-8789-601A0BD01F26}">
+    <comment ref="AG416" authorId="12" shapeId="0" xr:uid="{030E6257-8D2E-4479-8789-601A0BD01F26}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2761,7 +2797,7 @@
     Tic #1396</t>
       </text>
     </comment>
-    <comment ref="AH416" authorId="9" shapeId="0" xr:uid="{46D73F4D-7E18-4C6F-A359-B67B27630C06}">
+    <comment ref="AH416" authorId="13" shapeId="0" xr:uid="{46D73F4D-7E18-4C6F-A359-B67B27630C06}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2769,7 +2805,7 @@
     Additional mods for tic #1396</t>
       </text>
     </comment>
-    <comment ref="AR416" authorId="10" shapeId="0" xr:uid="{A80EFFA4-2C90-4EF2-ADD6-2ADCD79B8D2D}">
+    <comment ref="AR416" authorId="14" shapeId="0" xr:uid="{A80EFFA4-2C90-4EF2-ADD6-2ADCD79B8D2D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2975,7 +3011,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW419" authorId="11" shapeId="0" xr:uid="{D2E5511E-8ED7-4ED0-BB84-E99B393FD17C}">
+    <comment ref="AW419" authorId="15" shapeId="0" xr:uid="{D2E5511E-8ED7-4ED0-BB84-E99B393FD17C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2983,7 +3019,7 @@
     0.2 =&gt; 0.1 per Issue 396</t>
       </text>
     </comment>
-    <comment ref="AX419" authorId="12" shapeId="0" xr:uid="{98F0C951-CE30-40F1-B845-F787F3F6E92B}">
+    <comment ref="AX419" authorId="16" shapeId="0" xr:uid="{98F0C951-CE30-40F1-B845-F787F3F6E92B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2991,7 +3027,7 @@
     0.63 =&gt; 0.1 per Issue 396 Table 150.1-A</t>
       </text>
     </comment>
-    <comment ref="AW423" authorId="13" shapeId="0" xr:uid="{461F56F0-E5E3-4F00-B001-C7965D951317}">
+    <comment ref="AW423" authorId="17" shapeId="0" xr:uid="{461F56F0-E5E3-4F00-B001-C7965D951317}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2999,7 +3035,7 @@
     0.2 =&gt; 0.1 per Issue 396</t>
       </text>
     </comment>
-    <comment ref="AW424" authorId="14" shapeId="0" xr:uid="{268F927C-5C95-4F3A-BF87-1C6319A84546}">
+    <comment ref="AW424" authorId="18" shapeId="0" xr:uid="{268F927C-5C95-4F3A-BF87-1C6319A84546}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -3007,7 +3043,7 @@
     0.2 =&gt; 0.1 per Issue 396</t>
       </text>
     </comment>
-    <comment ref="AH430" authorId="15" shapeId="0" xr:uid="{9B97AB56-EB41-467D-B4FC-310C21C84424}">
+    <comment ref="AH430" authorId="19" shapeId="0" xr:uid="{9B97AB56-EB41-467D-B4FC-310C21C84424}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -3015,7 +3051,7 @@
     Tic #1396</t>
       </text>
     </comment>
-    <comment ref="AS430" authorId="16" shapeId="0" xr:uid="{1C13B9ED-440D-4C64-A02C-BC4A2615BB5C}">
+    <comment ref="AS430" authorId="20" shapeId="0" xr:uid="{1C13B9ED-440D-4C64-A02C-BC4A2615BB5C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -4270,7 +4306,7 @@
     <t>08/28/25 - SAC - mods updating WHFcfmdivisor for 2025+ code from 3 to 2 (gh dev #449) - also copied 2025 code rows down to create 2028 entries</t>
   </si>
   <si>
-    <t>8/30/25 - RJH - GitHub Issue #396: Modified 2025 SFam SteepRoofReflect and FlatRoofReflect</t>
+    <t>8/30/25 - RJH - GitHub Issue #396: Modified 2025 and 2028 SFam SteepRoofReflect and FlatRoofReflect</t>
   </si>
 </sst>
 </file>
@@ -5596,6 +5632,18 @@
   <threadedComment ref="AR383" dT="2025-03-31T19:31:30.60" personId="{CA85A688-6A1E-4293-B997-C12564BF5C8B}" id="{B702ED2D-EA27-4105-9F3D-EEB895251933}">
     <text>Tic #1396</text>
   </threadedComment>
+  <threadedComment ref="AW386" dT="2025-08-30T19:42:28.41" personId="{CA85A688-6A1E-4293-B997-C12564BF5C8B}" id="{5A2AFC92-DD15-4AE2-A916-B8A6D20139CD}">
+    <text>0.2 =&gt; 0.1 per Issue 396</text>
+  </threadedComment>
+  <threadedComment ref="AX386" dT="2025-08-30T19:44:53.84" personId="{CA85A688-6A1E-4293-B997-C12564BF5C8B}" id="{EC86CE9C-E40B-4C6A-A9B2-7780F895100E}">
+    <text>0.63 =&gt; 0.1 per Issue 396 Table 150.1-A</text>
+  </threadedComment>
+  <threadedComment ref="AW390" dT="2025-08-30T19:42:41.51" personId="{CA85A688-6A1E-4293-B997-C12564BF5C8B}" id="{CFBF76F3-508B-478A-AA3B-D827B9843997}">
+    <text>0.2 =&gt; 0.1 per Issue 396</text>
+  </threadedComment>
+  <threadedComment ref="AW391" dT="2025-08-30T19:42:49.27" personId="{CA85A688-6A1E-4293-B997-C12564BF5C8B}" id="{364B9DA7-9101-467F-9DFB-6A79815EFFAC}">
+    <text>0.2 =&gt; 0.1 per Issue 396</text>
+  </threadedComment>
   <threadedComment ref="AH397" dT="2025-03-31T19:32:27.51" personId="{CA85A688-6A1E-4293-B997-C12564BF5C8B}" id="{FC2E1ABC-F00F-493D-803C-4517A7E565B1}">
     <text>Tic #1396</text>
   </threadedComment>
@@ -5636,7 +5684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FF448"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
@@ -67211,11 +67259,11 @@
       <c r="AV386" s="27">
         <v>0</v>
       </c>
-      <c r="AW386" s="97">
-        <v>0.2</v>
-      </c>
-      <c r="AX386" s="97">
-        <v>0.63</v>
+      <c r="AW386" s="114">
+        <v>0.1</v>
+      </c>
+      <c r="AX386" s="114">
+        <v>0.1</v>
       </c>
       <c r="AY386" s="3" t="s">
         <v>116</v>
@@ -67724,8 +67772,8 @@
       <c r="AW388" s="27">
         <v>0.1</v>
       </c>
-      <c r="AX388" s="97">
-        <v>0.63</v>
+      <c r="AX388" s="114">
+        <v>0.1</v>
       </c>
       <c r="AY388" s="3" t="s">
         <v>116</v>
@@ -67978,8 +68026,8 @@
       <c r="AW389" s="27">
         <v>0.1</v>
       </c>
-      <c r="AX389" s="97">
-        <v>0.63</v>
+      <c r="AX389" s="114">
+        <v>0.1</v>
       </c>
       <c r="AY389" s="3" t="s">
         <v>116</v>
@@ -68229,11 +68277,11 @@
       <c r="AV390" s="27">
         <v>0</v>
       </c>
-      <c r="AW390" s="97">
-        <v>0.2</v>
-      </c>
-      <c r="AX390" s="97">
-        <v>0.63</v>
+      <c r="AW390" s="114">
+        <v>0.1</v>
+      </c>
+      <c r="AX390" s="114">
+        <v>0.1</v>
       </c>
       <c r="AY390" s="3" t="s">
         <v>116</v>
@@ -68483,11 +68531,11 @@
       <c r="AV391" s="27">
         <v>0</v>
       </c>
-      <c r="AW391" s="97">
-        <v>0.2</v>
-      </c>
-      <c r="AX391" s="97">
-        <v>0.63</v>
+      <c r="AW391" s="114">
+        <v>0.1</v>
+      </c>
+      <c r="AX391" s="114">
+        <v>0.1</v>
       </c>
       <c r="AY391" s="3" t="s">
         <v>116</v>
@@ -68741,8 +68789,8 @@
       <c r="AW392" s="27">
         <v>0.2</v>
       </c>
-      <c r="AX392" s="97">
-        <v>0.63</v>
+      <c r="AX392" s="114">
+        <v>0.1</v>
       </c>
       <c r="AY392" s="3" t="s">
         <v>116</v>
@@ -68996,8 +69044,8 @@
       <c r="AW393" s="27">
         <v>0.2</v>
       </c>
-      <c r="AX393" s="97">
-        <v>0.63</v>
+      <c r="AX393" s="114">
+        <v>0.1</v>
       </c>
       <c r="AY393" s="3" t="s">
         <v>116</v>
@@ -69251,8 +69299,8 @@
       <c r="AW394" s="27">
         <v>0.2</v>
       </c>
-      <c r="AX394" s="97">
-        <v>0.63</v>
+      <c r="AX394" s="114">
+        <v>0.1</v>
       </c>
       <c r="AY394" s="3" t="s">
         <v>116</v>
@@ -69761,8 +69809,8 @@
       <c r="AW396" s="27">
         <v>0.2</v>
       </c>
-      <c r="AX396" s="97">
-        <v>0.63</v>
+      <c r="AX396" s="114">
+        <v>0.1</v>
       </c>
       <c r="AY396" s="3" t="s">
         <v>116</v>

</xml_diff>